<commit_message>
fuck limit file size
</commit_message>
<xml_diff>
--- a/Scenario.xlsx
+++ b/Scenario.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20370"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7FD0CC-259E-4AA3-8750-CB5BF2B4E1B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9B6338-E562-4EDE-B7D2-962981BC3A34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmark" sheetId="1" r:id="rId1"/>
@@ -26,35 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="71">
   <si>
     <t>Benckmark4</t>
   </si>
   <si>
-    <t>DDPG_CL</t>
-  </si>
-  <si>
-    <t>Pop-CL</t>
-  </si>
-  <si>
-    <t>Benckmark5</t>
-  </si>
-  <si>
-    <t>Near-CL</t>
-  </si>
-  <si>
-    <t>DDPG_CA</t>
-  </si>
-  <si>
-    <t>Benckmark6</t>
-  </si>
-  <si>
-    <t>Benckmark7</t>
-  </si>
-  <si>
-    <t>Brute Force-CA</t>
-  </si>
-  <si>
     <t>Benchmark1</t>
   </si>
   <si>
@@ -64,12 +40,6 @@
     <t>Benchmark2</t>
   </si>
   <si>
-    <t>Benckmark3</t>
-  </si>
-  <si>
-    <t>Brute Force-CL</t>
-  </si>
-  <si>
     <t>Clustering Policy</t>
   </si>
   <si>
@@ -102,21 +72,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Optimal EE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Observation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[s2]
-g.real
-g.imag
-clustering_state
-caching_state
-reqStatistic_norm
-Req</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -128,23 +84,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[3]
-clustering_state
-caching_state
-reqStatistic_norm
-Req</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RL Best EE
-in EV phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Near-CL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>L</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -166,19 +105,6 @@
   </si>
   <si>
     <t>fixed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[s1]
-SINR
-clustering_state
-caching_state
-reqStatistic_norm
-Req</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Change/30 Itr</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -220,10 +146,6 @@
   </si>
   <si>
     <t>fixed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Makov</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -337,6 +259,82 @@
   </si>
   <si>
     <t>case: 40.10.50.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Benckmark3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SNR CL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POP CA 
+local cluster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POP CA 
+all AP the same</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DDPG_CL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DDPG_CA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[s2]***
+g.real
+g.imag
+clustering_state
+caching_state
+reqStatistic_norm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>change</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RL limited Connection?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ulimited</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DDPG 1act</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DDPG 2act</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BM1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L=2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BM2
+L=2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -458,14 +456,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="47" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="47" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3349,317 +3347,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>704849</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="圖片 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D13F19A-8E15-4BBE-B298-A3F5FF5433E5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7639050" y="28574"/>
-          <a:ext cx="4635500" cy="3476625"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>585786</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>413397</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>17153</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="圖片 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B951B361-3002-45D2-A3EC-264B89E8E224}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7629525" y="3386136"/>
-          <a:ext cx="4575822" cy="3431867"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>619125</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="10" name="直線單箭頭接點 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{086462BD-3516-4487-8A6F-A711B251C628}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6743700" y="5019675"/>
-          <a:ext cx="923925" cy="600075"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>962025</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>561975</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="13" name="直線單箭頭接點 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D60BAA53-7604-46B3-A6D7-635DDF463BCB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6724650" y="1362075"/>
-          <a:ext cx="923925" cy="600075"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>390524</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>528636</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>3175</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="圖片 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EDD4880-B41A-4B9A-8595-CA7F860E70FC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12182474" y="3328986"/>
-          <a:ext cx="4489451" cy="3367089"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>488950</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>500063</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="圖片 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03FB31F7-CBF4-4553-AA12-726D930B8301}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12280900" y="66675"/>
-          <a:ext cx="4311650" cy="3233738"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
@@ -3799,7 +3486,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4103,10 +3790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -4118,90 +3805,72 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" thickBot="1">
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="16.5" thickBot="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="29.25" thickBot="1">
       <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="6"/>
-    </row>
-    <row r="3" spans="1:3" ht="16.5" thickBot="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="29.25" thickBot="1">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1">
       <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickBot="1">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="16.5" thickBot="1">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="16.5" thickBot="1">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="16.5" thickBot="1">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>8</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="78.75">
+      <c r="A11" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="94.5">
+      <c r="A12" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4210,10 +3879,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2986BB-8F33-4471-B2CE-FA432FAA1E32}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -4226,46 +3895,59 @@
     <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="31.5">
+    <row r="1" spans="1:15" ht="31.5">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="H1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="78.75">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="94.5">
       <c r="A2">
         <v>4</v>
       </c>
@@ -4279,28 +3961,26 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>21</v>
+      <c r="H2" t="s">
+        <v>11</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2">
-        <v>141.21</v>
-      </c>
-      <c r="K2">
-        <v>142.16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="110.25">
+        <v>60</v>
+      </c>
+      <c r="J2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" ht="94.5">
       <c r="A3">
         <v>4</v>
       </c>
@@ -4313,99 +3993,90 @@
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="94.5">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="94.5">
+      <c r="A5">
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
         <v>21</v>
       </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3">
-        <v>132.91999999999999</v>
-      </c>
-      <c r="K3">
-        <v>142.16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="78.75">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4">
-        <v>132.91999999999999</v>
-      </c>
-      <c r="K4">
-        <v>142.16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="94.5">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>38</v>
+      <c r="H5" t="s">
+        <v>11</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5">
-        <v>127.57</v>
-      </c>
-      <c r="K5">
-        <v>142.16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="78.75">
+        <v>60</v>
+      </c>
+      <c r="J5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="94.5">
       <c r="A6">
         <v>40</v>
       </c>
@@ -4413,69 +4084,34 @@
         <v>10</v>
       </c>
       <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6">
         <v>5</v>
       </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
+      <c r="E6" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="G6" t="s">
         <v>21</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7">
-        <v>400</v>
-      </c>
-      <c r="B7">
-        <v>100</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="E8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
+        <v>60</v>
+      </c>
+      <c r="J6" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4504,49 +4140,49 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F1" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="G1" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="H1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="J1" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="K1" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="L1" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="M1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="63">
@@ -4563,22 +4199,22 @@
         <v>2</v>
       </c>
       <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="I2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="63">
@@ -4595,22 +4231,22 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="141.75">
@@ -4627,16 +4263,16 @@
         <v>5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="N4" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="126">
@@ -4653,13 +4289,13 @@
         <v>5</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="N5" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="O5">
         <v>28.488359462106601</v>
@@ -4679,24 +4315,24 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="126">
       <c r="E7" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -4722,44 +4358,44 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="63">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="B5" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="C6" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -4786,16 +4422,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4964,16 +4600,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5548,7 +5184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADC8946-7C3E-4BA7-848E-892B26A3208D}">
   <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
@@ -5562,18 +5198,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="B1" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -6017,97 +5653,97 @@
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="B47" s="7"/>
+      <c r="B47" s="5"/>
     </row>
     <row r="48" spans="1:3">
-      <c r="B48" s="7"/>
+      <c r="B48" s="5"/>
     </row>
     <row r="49" spans="2:2">
-      <c r="B49" s="7"/>
+      <c r="B49" s="5"/>
     </row>
     <row r="50" spans="2:2">
-      <c r="B50" s="7"/>
+      <c r="B50" s="5"/>
     </row>
     <row r="51" spans="2:2">
-      <c r="B51" s="7"/>
+      <c r="B51" s="5"/>
     </row>
     <row r="52" spans="2:2">
-      <c r="B52" s="7"/>
+      <c r="B52" s="5"/>
     </row>
     <row r="53" spans="2:2">
-      <c r="B53" s="7"/>
+      <c r="B53" s="5"/>
     </row>
     <row r="54" spans="2:2">
-      <c r="B54" s="7"/>
+      <c r="B54" s="5"/>
     </row>
     <row r="55" spans="2:2">
-      <c r="B55" s="7"/>
+      <c r="B55" s="5"/>
     </row>
     <row r="56" spans="2:2">
-      <c r="B56" s="7"/>
+      <c r="B56" s="5"/>
     </row>
     <row r="57" spans="2:2">
-      <c r="B57" s="7"/>
+      <c r="B57" s="5"/>
     </row>
     <row r="58" spans="2:2">
-      <c r="B58" s="7"/>
+      <c r="B58" s="5"/>
     </row>
     <row r="59" spans="2:2">
-      <c r="B59" s="7"/>
+      <c r="B59" s="5"/>
     </row>
     <row r="60" spans="2:2">
-      <c r="B60" s="7"/>
+      <c r="B60" s="5"/>
     </row>
     <row r="61" spans="2:2">
-      <c r="B61" s="7"/>
+      <c r="B61" s="5"/>
     </row>
     <row r="62" spans="2:2">
-      <c r="B62" s="7"/>
+      <c r="B62" s="5"/>
     </row>
     <row r="63" spans="2:2">
-      <c r="B63" s="7"/>
+      <c r="B63" s="5"/>
     </row>
     <row r="64" spans="2:2">
-      <c r="B64" s="7"/>
+      <c r="B64" s="5"/>
     </row>
     <row r="65" spans="2:2">
-      <c r="B65" s="7"/>
+      <c r="B65" s="5"/>
     </row>
     <row r="66" spans="2:2">
-      <c r="B66" s="7"/>
+      <c r="B66" s="5"/>
     </row>
     <row r="67" spans="2:2">
-      <c r="B67" s="7"/>
+      <c r="B67" s="5"/>
     </row>
     <row r="68" spans="2:2">
-      <c r="B68" s="7"/>
+      <c r="B68" s="5"/>
     </row>
     <row r="69" spans="2:2">
-      <c r="B69" s="7"/>
+      <c r="B69" s="5"/>
     </row>
     <row r="70" spans="2:2">
-      <c r="B70" s="7"/>
+      <c r="B70" s="5"/>
     </row>
     <row r="71" spans="2:2">
-      <c r="B71" s="7"/>
+      <c r="B71" s="5"/>
     </row>
     <row r="72" spans="2:2">
-      <c r="B72" s="7"/>
+      <c r="B72" s="5"/>
     </row>
     <row r="73" spans="2:2">
-      <c r="B73" s="7"/>
+      <c r="B73" s="5"/>
     </row>
     <row r="74" spans="2:2">
-      <c r="B74" s="7"/>
+      <c r="B74" s="5"/>
     </row>
     <row r="75" spans="2:2">
-      <c r="B75" s="7"/>
+      <c r="B75" s="5"/>
     </row>
     <row r="76" spans="2:2">
-      <c r="B76" s="7"/>
+      <c r="B76" s="5"/>
     </row>
     <row r="77" spans="2:2">
-      <c r="B77" s="7"/>
+      <c r="B77" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>